<commit_message>
final results for simulated data
</commit_message>
<xml_diff>
--- a/paper/tables/simulation_parameters.xlsx
+++ b/paper/tables/simulation_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1d0f8721c60e9a63/GAU/3. Semester/Statistisches Praktikum/Git/NEW_Ensemble_Techniques_TS_FC/paper/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D53C5DDC-65EC-49EE-B32D-48576E73124C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="163" documentId="8_{D53C5DDC-65EC-49EE-B32D-48576E73124C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C454852F-E6A8-4185-B98A-CB39E6718EFD}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C3EF23BD-2587-49A3-9C66-8DE91B20914D}"/>
+    <workbookView xWindow="-24398" yWindow="-2422" windowWidth="24496" windowHeight="16395" xr2:uid="{C3EF23BD-2587-49A3-9C66-8DE91B20914D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
   <si>
     <t>Descrption</t>
   </si>
@@ -45,16 +45,154 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
+  <si>
+    <t>alpha (AR)</t>
+  </si>
+  <si>
+    <t>gamma (MA)</t>
+  </si>
+  <si>
+    <t>theta (SAR)</t>
+  </si>
+  <si>
+    <t>phi SMA</t>
+  </si>
+  <si>
+    <t>beta X</t>
+  </si>
+  <si>
+    <t>sigma2</t>
+  </si>
+  <si>
+    <t>RW</t>
+  </si>
+  <si>
+    <t>TrendSeasRW</t>
+  </si>
+  <si>
+    <t>WeakSARIMA</t>
+  </si>
+  <si>
+    <t>StrongSARIMA</t>
+  </si>
+  <si>
+    <t>SARIMAX</t>
+  </si>
+  <si>
+    <t>Random Walk</t>
+  </si>
+  <si>
+    <t>Seasonal Autoregressive Integrated Moving Average</t>
+  </si>
+  <si>
+    <t>Random Walk + Seasonality + Trend</t>
+  </si>
+  <si>
+    <t>Seasonal Autoregressive Integrated Moving Average with covariate influence</t>
+  </si>
+  <si>
+    <t>Seasonal Autoregressive Integrated Moving Average with more lags and pattern</t>
+  </si>
+  <si>
+    <t>ARIMA(0,1,0)</t>
+  </si>
+  <si>
+    <t>SARIMA(0,1,0)(1,0,0)_12</t>
+  </si>
+  <si>
+    <t>Exo1</t>
+  </si>
+  <si>
+    <t>Exo2</t>
+  </si>
+  <si>
+    <t>Exo3</t>
+  </si>
+  <si>
+    <t>Exogenous Variable 1</t>
+  </si>
+  <si>
+    <t>Exogenous Variable 2</t>
+  </si>
+  <si>
+    <t>Exogenous Variable 3</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>SARIMA(1,1,1)(2,0,0)_12</t>
+  </si>
+  <si>
+    <t>[0.4, 0.3]'</t>
+  </si>
+  <si>
+    <t>SARIMA(3,1,4)(2,0,1)_12</t>
+  </si>
+  <si>
+    <t>[0.6, -0.2, 0.1]'</t>
+  </si>
+  <si>
+    <t>[0.4, -0.2, -0.1, 0.1]'</t>
+  </si>
+  <si>
+    <t>SARIMIAX(3,1,4)(2,0,1)_12 + betaX</t>
+  </si>
+  <si>
+    <t>[0.1, 0.025, 0..01]'</t>
+  </si>
+  <si>
+    <t>[0.05, 0.01]'</t>
+  </si>
+  <si>
+    <t>SARIMA(1,1,3)(2,0,0)_12</t>
+  </si>
+  <si>
+    <t>SARIMA(4,1,4)(1,0,0)_12</t>
+  </si>
+  <si>
+    <t>[0.05, 0.05, -0.1, 0.1]'</t>
+  </si>
+  <si>
+    <t>[0.1, 0.01, -0.2, -0.1]'</t>
+  </si>
+  <si>
+    <t>SARIMA(3,1,1)(2,0,1)_12</t>
+  </si>
+  <si>
+    <t>[0.15, -0.01, -0.01]'</t>
+  </si>
+  <si>
+    <t>[0.3, 0.2]'</t>
+  </si>
+  <si>
+    <t>upper</t>
+  </si>
+  <si>
+    <t>lower</t>
+  </si>
+  <si>
+    <t>[0.4, 0.2, -0.3]'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -80,8 +218,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,13 +557,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91563E6D-0CAE-4E1F-B106-03A3649E34A0}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K10" sqref="K2:K10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -432,8 +583,351 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1">
+        <v>40</v>
+      </c>
+      <c r="L2" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1">
+        <v>40</v>
+      </c>
+      <c r="L3" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1">
+        <v>40</v>
+      </c>
+      <c r="L4" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="1">
+        <v>-0.2</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1">
+        <v>40</v>
+      </c>
+      <c r="L5" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="1">
+        <v>-0.2</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1">
+        <v>40</v>
+      </c>
+      <c r="L6" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E8" s="1">
+        <v>-0.2</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="1">
+        <v>100</v>
+      </c>
+      <c r="K8" s="1">
+        <v>200</v>
+      </c>
+      <c r="L8" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="K9" s="1">
+        <v>40</v>
+      </c>
+      <c r="L9" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="1">
+        <v>-0.05</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="1">
+        <v>-0.2</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" s="1">
+        <v>4</v>
+      </c>
+      <c r="K10" s="1">
+        <v>900</v>
+      </c>
+      <c r="L10" s="1">
+        <v>950</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>